<commit_message>
Added excel for units with abilities
</commit_message>
<xml_diff>
--- a/Documentation/Units.xlsx
+++ b/Documentation/Units.xlsx
@@ -9,10 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8832"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8832" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="160">
   <si>
     <t>Base Class</t>
   </si>
@@ -417,6 +420,93 @@
   </si>
   <si>
     <t>Gives a enemie  x% less maxHp for y seconds every z seconds</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Required tech</t>
+  </si>
+  <si>
+    <t>Upgrade from building</t>
+  </si>
+  <si>
+    <t>Gains 10% extra damage for every 10% of hp lost</t>
+  </si>
+  <si>
+    <t>Every attack against this unit returns 30% damage</t>
+  </si>
+  <si>
+    <t>Hits all enemies within 1 range of the target for 30% percent damage</t>
+  </si>
+  <si>
+    <t>Hits all enemies around the target within 1 range for 20% percent</t>
+  </si>
+  <si>
+    <t>Gives allies within 2 range 25% extra hp and 25% extra damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gives enemies within 3 range 15% less maxHp </t>
+  </si>
+  <si>
+    <t>Gives enemies within 3 range 15% less damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summons a random tier 2 unit every 32 ticks for 60 ticks </t>
+  </si>
+  <si>
+    <t>Every 20 ticks a unit that died in the last 40 ticks can be revived for 40 ticks with 30% stats</t>
+  </si>
+  <si>
+    <t>Shotgun</t>
+  </si>
+  <si>
+    <t>Hits 6 enemies within range</t>
+  </si>
+  <si>
+    <t>Hits 2 enemies within range</t>
+  </si>
+  <si>
+    <t>Ticks per attack</t>
+  </si>
+  <si>
+    <t>armor</t>
+  </si>
+  <si>
+    <t>heals a friendly unit for 8 health every 4 ticks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gives an ally 25% extra max hp and 25% extra damage for 40 ticks every 20 ticks </t>
+  </si>
+  <si>
+    <t>Gives a enemy  25% less maxHp and 25% less damage for 40 ticks every 20 ticks</t>
+  </si>
+  <si>
+    <t>Summons a base unit every 12 ticks</t>
+  </si>
+  <si>
+    <t>Every attack converts 25% of the damage done to life for this unit</t>
+  </si>
+  <si>
+    <t>heals all units within 2 range for 4 every 4 ticks</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Required id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>required</t>
   </si>
 </sst>
 </file>
@@ -751,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2207,4 +2297,4232 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:Q32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" t="s">
+        <v>129</v>
+      </c>
+      <c r="P1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>40</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>H2*J2</f>
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <f>IF(J2=0,0,1/J2*4)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>160</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>12</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K32" si="0">H3*J3</f>
+        <v>12</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L32" si="1">IF(J3=0,0,1/J3*4)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>80</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>16</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>80</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M5" t="s">
+        <v>148</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>640</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>240</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>32</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>400</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>16</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="F9">
+        <v>80</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>120</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>0.25</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>160</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>16</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>120</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>12</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M11" t="s">
+        <v>145</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12">
+        <v>50</v>
+      </c>
+      <c r="F12">
+        <v>120</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12" t="s">
+        <v>149</v>
+      </c>
+      <c r="N12">
+        <v>25</v>
+      </c>
+      <c r="O12">
+        <v>25</v>
+      </c>
+      <c r="P12">
+        <v>10</v>
+      </c>
+      <c r="Q12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13">
+        <v>50</v>
+      </c>
+      <c r="F13">
+        <v>120</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
+        <v>150</v>
+      </c>
+      <c r="N13">
+        <v>25</v>
+      </c>
+      <c r="O13">
+        <v>25</v>
+      </c>
+      <c r="P13">
+        <v>10</v>
+      </c>
+      <c r="Q13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+      <c r="F14">
+        <v>120</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
+        <v>151</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15">
+        <v>250</v>
+      </c>
+      <c r="F15">
+        <v>640</v>
+      </c>
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <v>32</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M15" t="s">
+        <v>152</v>
+      </c>
+      <c r="N15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16">
+        <v>250</v>
+      </c>
+      <c r="F16">
+        <v>640</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>32</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M16" t="s">
+        <v>134</v>
+      </c>
+      <c r="N16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17">
+        <v>250</v>
+      </c>
+      <c r="F17">
+        <v>1400</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M17" t="s">
+        <v>135</v>
+      </c>
+      <c r="N17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18">
+        <v>250</v>
+      </c>
+      <c r="F18">
+        <v>1400</v>
+      </c>
+      <c r="G18">
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>16</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19">
+        <v>250</v>
+      </c>
+      <c r="F19">
+        <v>240</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>200</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0.5</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20">
+        <v>250</v>
+      </c>
+      <c r="F20">
+        <v>400</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>40</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M20" t="s">
+        <v>136</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21">
+        <v>250</v>
+      </c>
+      <c r="F21">
+        <v>120</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>120</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <v>0.25</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="M21" t="s">
+        <v>137</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22">
+        <v>250</v>
+      </c>
+      <c r="F22">
+        <v>120</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>320</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+      <c r="J22">
+        <v>0.25</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>143</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23">
+        <v>250</v>
+      </c>
+      <c r="F23">
+        <v>240</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>24</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M23" t="s">
+        <v>144</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="1">
+        <v>250</v>
+      </c>
+      <c r="F24" s="1">
+        <v>160</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1">
+        <v>32</v>
+      </c>
+      <c r="I24" s="1">
+        <v>2</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25">
+        <v>250</v>
+      </c>
+      <c r="F25">
+        <v>200</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>16</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="1">
+        <v>250</v>
+      </c>
+      <c r="F26" s="1">
+        <v>200</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>4</v>
+      </c>
+      <c r="I26" s="1">
+        <v>2</v>
+      </c>
+      <c r="J26" s="1">
+        <v>4</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27">
+        <v>250</v>
+      </c>
+      <c r="F27">
+        <v>120</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M27" t="s">
+        <v>153</v>
+      </c>
+      <c r="N27">
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28">
+        <v>250</v>
+      </c>
+      <c r="F28">
+        <v>120</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M28" t="s">
+        <v>138</v>
+      </c>
+      <c r="N28">
+        <v>2</v>
+      </c>
+      <c r="O28">
+        <v>25</v>
+      </c>
+      <c r="P28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29">
+        <v>250</v>
+      </c>
+      <c r="F29">
+        <v>120</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M29" t="s">
+        <v>139</v>
+      </c>
+      <c r="N29">
+        <v>3</v>
+      </c>
+      <c r="O29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30">
+        <v>250</v>
+      </c>
+      <c r="F30">
+        <v>120</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M30" t="s">
+        <v>140</v>
+      </c>
+      <c r="N30">
+        <v>3</v>
+      </c>
+      <c r="O30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31">
+        <v>250</v>
+      </c>
+      <c r="F31">
+        <v>120</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M31" t="s">
+        <v>141</v>
+      </c>
+      <c r="N31">
+        <v>8</v>
+      </c>
+      <c r="O31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="1">
+        <v>250</v>
+      </c>
+      <c r="F32" s="1">
+        <v>120</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>2</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="N32" s="1">
+        <v>5</v>
+      </c>
+      <c r="O32" s="1">
+        <v>10</v>
+      </c>
+      <c r="P32" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N32"/>
+  <sheetViews>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A1:N32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="16.44140625" customWidth="1"/>
+    <col min="14" max="14" width="79.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>146</v>
+      </c>
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2">
+        <f>SUMIF(B:B,C2,A:A)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>40</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f>I2*K2</f>
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <f>IF(K2=0,0,1/K2*4)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D32" si="0">SUMIF(B:B,C3,A:A)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>160</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L32" si="1">I3*K3</f>
+        <v>12</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M32" si="2">IF(K3=0,0,1/K3*4)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" ref="A4:A32" si="3">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>80</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>80</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>640</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
+      <c r="G7">
+        <v>240</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>32</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+      <c r="G8">
+        <v>400</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>16</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9">
+        <v>80</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>120</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>0.25</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10">
+        <v>160</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>16</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11">
+        <v>50</v>
+      </c>
+      <c r="G11">
+        <v>120</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>12</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12">
+        <v>120</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="G13">
+        <v>120</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14">
+        <v>50</v>
+      </c>
+      <c r="G14">
+        <v>120</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15">
+        <v>250</v>
+      </c>
+      <c r="G15">
+        <v>640</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>32</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16">
+        <v>250</v>
+      </c>
+      <c r="G16">
+        <v>640</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>32</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17">
+        <v>250</v>
+      </c>
+      <c r="G17">
+        <v>1400</v>
+      </c>
+      <c r="H17">
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <v>16</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18">
+        <v>250</v>
+      </c>
+      <c r="G18">
+        <v>1400</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>16</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19">
+        <v>250</v>
+      </c>
+      <c r="G19">
+        <v>240</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>200</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0.5</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20">
+        <v>250</v>
+      </c>
+      <c r="G20">
+        <v>400</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>40</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21">
+        <v>250</v>
+      </c>
+      <c r="G21">
+        <v>120</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>120</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21">
+        <v>0.25</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="N21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22">
+        <v>250</v>
+      </c>
+      <c r="G22">
+        <v>120</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>320</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+      <c r="K22">
+        <v>0.25</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23">
+        <v>250</v>
+      </c>
+      <c r="G23">
+        <v>240</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>24</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="1">
+        <v>250</v>
+      </c>
+      <c r="G24" s="1">
+        <v>160</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1">
+        <v>32</v>
+      </c>
+      <c r="J24" s="1">
+        <v>2</v>
+      </c>
+      <c r="K24" s="1">
+        <v>1</v>
+      </c>
+      <c r="L24" s="1">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25">
+        <v>250</v>
+      </c>
+      <c r="G25">
+        <v>200</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>16</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="1">
+        <v>250</v>
+      </c>
+      <c r="G26" s="1">
+        <v>200</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>4</v>
+      </c>
+      <c r="J26" s="1">
+        <v>2</v>
+      </c>
+      <c r="K26" s="1">
+        <v>4</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27">
+        <v>250</v>
+      </c>
+      <c r="G27">
+        <v>120</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28">
+        <v>250</v>
+      </c>
+      <c r="G28">
+        <v>120</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29">
+        <v>250</v>
+      </c>
+      <c r="G29">
+        <v>120</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30">
+        <v>250</v>
+      </c>
+      <c r="G30">
+        <v>120</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E31" t="s">
+        <v>96</v>
+      </c>
+      <c r="F31">
+        <v>250</v>
+      </c>
+      <c r="G31">
+        <v>120</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32" s="1">
+        <v>250</v>
+      </c>
+      <c r="G32" s="1">
+        <v>120</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1">
+        <v>2</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A27" activeCellId="2" sqref="A1:K23 A25:K25 A27:K31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>40</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>160</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" ref="A4:A32" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <v>80</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5">
+        <v>80</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>640</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>240</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>32</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8">
+        <v>400</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>16</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>80</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>120</v>
+      </c>
+      <c r="J9">
+        <v>16</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10">
+        <v>160</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>16</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>120</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>12</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12">
+        <v>120</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13">
+        <v>120</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14">
+        <v>120</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>250</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15">
+        <v>640</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>32</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16">
+        <v>250</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16">
+        <v>640</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>32</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>250</v>
+      </c>
+      <c r="D17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17">
+        <v>1400</v>
+      </c>
+      <c r="H17">
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <v>16</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>250</v>
+      </c>
+      <c r="D18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18">
+        <v>1400</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>16</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>250</v>
+      </c>
+      <c r="D19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19">
+        <v>240</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>200</v>
+      </c>
+      <c r="J19">
+        <v>8</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>250</v>
+      </c>
+      <c r="D20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20">
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20">
+        <v>400</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>40</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>250</v>
+      </c>
+      <c r="D21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21">
+        <v>120</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>120</v>
+      </c>
+      <c r="J21">
+        <v>16</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="L21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>250</v>
+      </c>
+      <c r="D22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22">
+        <v>120</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>320</v>
+      </c>
+      <c r="J22">
+        <v>16</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23">
+        <v>250</v>
+      </c>
+      <c r="D23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>143</v>
+      </c>
+      <c r="G23">
+        <v>240</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>24</v>
+      </c>
+      <c r="J23">
+        <v>4</v>
+      </c>
+      <c r="K23">
+        <v>2</v>
+      </c>
+      <c r="L23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="1">
+        <v>250</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="1">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="1">
+        <v>160</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1">
+        <v>32</v>
+      </c>
+      <c r="J24" s="1">
+        <v>4</v>
+      </c>
+      <c r="K24" s="1">
+        <v>2</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>250</v>
+      </c>
+      <c r="D25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25">
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25">
+        <v>200</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>16</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="1">
+        <v>250</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="1">
+        <v>9</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G26" s="1">
+        <v>200</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>4</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1">
+        <v>2</v>
+      </c>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <v>250</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27">
+        <v>120</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>2</v>
+      </c>
+      <c r="L27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28">
+        <v>250</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28">
+        <v>11</v>
+      </c>
+      <c r="F28" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28">
+        <v>120</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>2</v>
+      </c>
+      <c r="L28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29">
+        <v>250</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>74</v>
+      </c>
+      <c r="G29">
+        <v>120</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>2</v>
+      </c>
+      <c r="L29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30">
+        <v>250</v>
+      </c>
+      <c r="D30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30">
+        <v>12</v>
+      </c>
+      <c r="F30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30">
+        <v>120</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>2</v>
+      </c>
+      <c r="L30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31">
+        <v>250</v>
+      </c>
+      <c r="D31" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31">
+        <v>13</v>
+      </c>
+      <c r="F31" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31">
+        <v>120</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>2</v>
+      </c>
+      <c r="L31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="1">
+        <v>250</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="1">
+        <v>13</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" s="1">
+        <v>120</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <v>2</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>